<commit_message>
updating calculate_salary, still have bug on timekeeping
</commit_message>
<xml_diff>
--- a/test_salary.xlsx
+++ b/test_salary.xlsx
@@ -4,18 +4,31 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12330"/>
+    <workbookView windowHeight="17260"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="RD" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="13">
   <si>
     <t>uuid</t>
   </si>
@@ -38,6 +51,15 @@
     <t>Alice Smith</t>
   </si>
   <si>
+    <t>ID2</t>
+  </si>
+  <si>
+    <t>Bob Johnson</t>
+  </si>
+  <si>
+    <t>abs</t>
+  </si>
+  <si>
     <t>date</t>
   </si>
   <si>
@@ -50,19 +72,19 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
   <numFmts count="5">
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="176" formatCode="yyyy/m/d\ h:mm:ss"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="180" formatCode="yyyy/m/d\ h:mm:ss"/>
   </numFmts>
   <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -82,7 +104,7 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -90,14 +112,14 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -105,7 +127,7 @@
       <b/>
       <sz val="18"/>
       <color theme="3"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -113,7 +135,7 @@
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -121,7 +143,7 @@
       <b/>
       <sz val="15"/>
       <color theme="3"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -129,7 +151,7 @@
       <b/>
       <sz val="13"/>
       <color theme="3"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -137,14 +159,14 @@
       <b/>
       <sz val="11"/>
       <color theme="3"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -152,7 +174,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -160,7 +182,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -168,14 +190,14 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -183,52 +205,58 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -526,19 +554,19 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="178" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -547,7 +575,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -571,16 +599,16 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -589,100 +617,100 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="58" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -691,23 +719,20 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="58" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="35" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="21" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -715,63 +740,69 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="21" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="35" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="35" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="千位分隔" xfId="1" builtinId="3"/>
-    <cellStyle name="货币" xfId="2" builtinId="4"/>
-    <cellStyle name="百分比" xfId="3" builtinId="5"/>
-    <cellStyle name="千位分隔[0]" xfId="4" builtinId="6"/>
-    <cellStyle name="货币[0]" xfId="5" builtinId="7"/>
-    <cellStyle name="超链接" xfId="6" builtinId="8"/>
-    <cellStyle name="已访问的超链接" xfId="7" builtinId="9"/>
-    <cellStyle name="注释" xfId="8" builtinId="10"/>
-    <cellStyle name="警告文本" xfId="9" builtinId="11"/>
-    <cellStyle name="标题" xfId="10" builtinId="15"/>
-    <cellStyle name="解释性文本" xfId="11" builtinId="53"/>
-    <cellStyle name="标题 1" xfId="12" builtinId="16"/>
-    <cellStyle name="标题 2" xfId="13" builtinId="17"/>
-    <cellStyle name="标题 3" xfId="14" builtinId="18"/>
-    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
-    <cellStyle name="输入" xfId="16" builtinId="20"/>
-    <cellStyle name="输出" xfId="17" builtinId="21"/>
-    <cellStyle name="计算" xfId="18" builtinId="22"/>
-    <cellStyle name="检查单元格" xfId="19" builtinId="23"/>
-    <cellStyle name="链接单元格" xfId="20" builtinId="24"/>
-    <cellStyle name="汇总" xfId="21" builtinId="25"/>
-    <cellStyle name="好" xfId="22" builtinId="26"/>
-    <cellStyle name="差" xfId="23" builtinId="27"/>
-    <cellStyle name="适中" xfId="24" builtinId="28"/>
-    <cellStyle name="强调文字颜色 1" xfId="25" builtinId="29"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="26" builtinId="30"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="27" builtinId="31"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="28" builtinId="32"/>
-    <cellStyle name="强调文字颜色 2" xfId="29" builtinId="33"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="30" builtinId="34"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="31" builtinId="35"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="32" builtinId="36"/>
-    <cellStyle name="强调文字颜色 3" xfId="33" builtinId="37"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="34" builtinId="38"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="35" builtinId="39"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="36" builtinId="40"/>
-    <cellStyle name="强调文字颜色 4" xfId="37" builtinId="41"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="38" builtinId="42"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="39" builtinId="43"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="40" builtinId="44"/>
-    <cellStyle name="强调文字颜色 5" xfId="41" builtinId="45"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="42" builtinId="46"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="43" builtinId="47"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="44" builtinId="48"/>
-    <cellStyle name="强调文字颜色 6" xfId="45" builtinId="49"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="46" builtinId="50"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
+    <cellStyle name="Percent" xfId="3" builtinId="5"/>
+    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
+    <cellStyle name="Note" xfId="8" builtinId="10"/>
+    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
+    <cellStyle name="Title" xfId="10" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="11" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="12" builtinId="16"/>
+    <cellStyle name="Heading 2" xfId="13" builtinId="17"/>
+    <cellStyle name="Heading 3" xfId="14" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="15" builtinId="19"/>
+    <cellStyle name="Input" xfId="16" builtinId="20"/>
+    <cellStyle name="Output" xfId="17" builtinId="21"/>
+    <cellStyle name="Calculation" xfId="18" builtinId="22"/>
+    <cellStyle name="Check Cell" xfId="19" builtinId="23"/>
+    <cellStyle name="Linked Cell" xfId="20" builtinId="24"/>
+    <cellStyle name="Total" xfId="21" builtinId="25"/>
+    <cellStyle name="Good" xfId="22" builtinId="26"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="24" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - Accent1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - Accent1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - Accent1" xfId="28" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - Accent2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - Accent2" xfId="32" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - Accent3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
+    <cellStyle name="Accent4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - Accent4" xfId="40" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - Accent5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - Accent5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="44" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1069,22 +1100,22 @@
   <sheetPr codeName="Sheet1">
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:H32"/>
+  <dimension ref="A1:H64"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="F61" sqref="F61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="7"/>
   <cols>
-    <col min="1" max="1" width="12.4333333333333" style="11" customWidth="1"/>
-    <col min="2" max="2" width="10.7166666666667" style="2" customWidth="1"/>
-    <col min="3" max="3" width="18.0083333333333" style="12" customWidth="1"/>
-    <col min="4" max="4" width="18.15" style="12" customWidth="1"/>
-    <col min="5" max="5" width="20.575" style="12" customWidth="1"/>
-    <col min="6" max="6" width="12.4333333333333" style="13" customWidth="1"/>
-    <col min="7" max="7" width="11.4333333333333" style="13" customWidth="1"/>
-    <col min="8" max="8" width="10.2916666666667" style="13" customWidth="1"/>
+    <col min="1" max="1" width="12.4296875" style="11" customWidth="1"/>
+    <col min="2" max="2" width="10.71875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="18.0078125" style="12" customWidth="1"/>
+    <col min="4" max="4" width="18.1484375" style="12" customWidth="1"/>
+    <col min="5" max="5" width="20.578125" style="12" customWidth="1"/>
+    <col min="6" max="6" width="12.4296875" style="13" customWidth="1"/>
+    <col min="7" max="7" width="11.4296875" style="13" customWidth="1"/>
+    <col min="8" max="8" width="10.2890625" style="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="17.25" customHeight="1" spans="1:8">
@@ -1103,541 +1134,1074 @@
       <c r="E1" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:8">
-      <c r="A2" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="19">
+      <c r="A2" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="18">
         <v>45474.375</v>
       </c>
-      <c r="D2" s="19"/>
+      <c r="D2" s="18"/>
       <c r="E2" s="10"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
     </row>
     <row r="3" ht="17.25" customHeight="1" spans="1:6">
-      <c r="A3" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="19">
+      <c r="A3" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="18">
         <f t="shared" ref="C3:C23" si="0">C2+1</f>
         <v>45475.375</v>
       </c>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="16"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="20"/>
     </row>
     <row r="4" ht="17.25" customHeight="1" spans="1:5">
-      <c r="A4" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="19">
+      <c r="A4" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="18">
         <f t="shared" si="0"/>
         <v>45476.375</v>
       </c>
-      <c r="D4" s="19">
+      <c r="D4" s="18">
         <v>45476.3888888889</v>
       </c>
-      <c r="E4" s="19">
+      <c r="E4" s="18">
         <v>45476.7083333333</v>
       </c>
     </row>
     <row r="5" ht="17.25" customHeight="1" spans="1:5">
-      <c r="A5" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="19">
+      <c r="A5" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="18">
         <f t="shared" si="0"/>
         <v>45477.375</v>
       </c>
-      <c r="D5" s="19">
+      <c r="D5" s="18">
         <v>45477.375</v>
       </c>
-      <c r="E5" s="19">
+      <c r="E5" s="18">
         <v>45477.7083333333</v>
       </c>
     </row>
     <row r="6" ht="17.25" customHeight="1" spans="1:5">
-      <c r="A6" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="19">
+      <c r="A6" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="18">
         <f t="shared" si="0"/>
         <v>45478.375</v>
       </c>
-      <c r="D6" s="19">
+      <c r="D6" s="18">
         <v>45478.375</v>
       </c>
-      <c r="E6" s="19">
+      <c r="E6" s="18">
         <v>45478.7083333333</v>
       </c>
     </row>
     <row r="7" ht="17.25" customHeight="1" spans="1:5">
-      <c r="A7" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="19">
+      <c r="A7" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="18">
         <f t="shared" si="0"/>
         <v>45479.375</v>
       </c>
-      <c r="D7" s="19">
+      <c r="D7" s="18">
         <v>45479.5</v>
       </c>
-      <c r="E7" s="19">
+      <c r="E7" s="18">
         <v>45479.7083333333</v>
       </c>
     </row>
-    <row r="8" ht="15" spans="1:5">
-      <c r="A8" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="19">
+    <row r="8" spans="1:5">
+      <c r="A8" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="18">
         <f t="shared" si="0"/>
         <v>45480.375</v>
       </c>
-      <c r="D8" s="19"/>
+      <c r="D8" s="18"/>
       <c r="E8" s="10"/>
     </row>
-    <row r="9" ht="15" spans="1:5">
-      <c r="A9" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="19">
+    <row r="9" spans="1:5">
+      <c r="A9" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="18">
         <f t="shared" si="0"/>
         <v>45481.375</v>
       </c>
-      <c r="D9" s="19">
+      <c r="D9" s="18">
         <v>45481.375</v>
       </c>
-      <c r="E9" s="19">
+      <c r="E9" s="18">
         <v>45481.7083333333</v>
       </c>
     </row>
-    <row r="10" ht="15" spans="1:5">
-      <c r="A10" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" s="19">
+    <row r="10" spans="1:5">
+      <c r="A10" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="18">
         <f t="shared" si="0"/>
         <v>45482.375</v>
       </c>
-      <c r="D10" s="19">
+      <c r="D10" s="18">
         <v>45482.375</v>
       </c>
-      <c r="E10" s="19">
+      <c r="E10" s="18">
         <v>45482.7083333333</v>
       </c>
     </row>
-    <row r="11" ht="15" spans="1:5">
-      <c r="A11" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" s="19">
+    <row r="11" spans="1:5">
+      <c r="A11" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="18">
         <f t="shared" si="0"/>
         <v>45483.375</v>
       </c>
-      <c r="D11" s="19">
+      <c r="D11" s="18">
         <v>45483.375</v>
       </c>
-      <c r="E11" s="19">
+      <c r="E11" s="18">
         <v>45483.7083333333</v>
       </c>
     </row>
-    <row r="12" ht="15" spans="1:5">
-      <c r="A12" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="B12" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" s="19">
+    <row r="12" spans="1:5">
+      <c r="A12" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="18">
         <f t="shared" si="0"/>
         <v>45484.375</v>
       </c>
-      <c r="D12" s="19">
+      <c r="D12" s="18">
         <v>45484.375</v>
       </c>
-      <c r="E12" s="19">
+      <c r="E12" s="18">
         <v>45484.7083333333</v>
       </c>
     </row>
-    <row r="13" ht="15" spans="1:5">
-      <c r="A13" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="B13" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" s="19">
+    <row r="13" spans="1:5">
+      <c r="A13" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="18">
         <f t="shared" si="0"/>
         <v>45485.375</v>
       </c>
-      <c r="D13" s="19">
+      <c r="D13" s="18">
         <v>45485.375</v>
       </c>
-      <c r="E13" s="19">
+      <c r="E13" s="18">
         <v>45485.7083333333</v>
       </c>
     </row>
-    <row r="14" ht="15" spans="1:5">
-      <c r="A14" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="B14" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="C14" s="19">
+    <row r="14" spans="1:5">
+      <c r="A14" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="18">
         <f t="shared" si="0"/>
         <v>45486.375</v>
       </c>
-      <c r="D14" s="19">
+      <c r="D14" s="18">
         <v>45486.375</v>
       </c>
-      <c r="E14" s="19">
+      <c r="E14" s="18">
         <v>45486.7083333333</v>
       </c>
     </row>
-    <row r="15" ht="15" spans="1:5">
-      <c r="A15" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="B15" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15" s="19">
+    <row r="15" spans="1:5">
+      <c r="A15" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="18">
         <f t="shared" si="0"/>
         <v>45487.375</v>
       </c>
-      <c r="D15" s="19">
+      <c r="D15" s="18">
         <v>45487.375</v>
       </c>
-      <c r="E15" s="19">
+      <c r="E15" s="18">
         <v>45487.7083333333</v>
       </c>
     </row>
-    <row r="16" ht="15" spans="1:5">
-      <c r="A16" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="B16" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="C16" s="19">
+    <row r="16" spans="1:5">
+      <c r="A16" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="18">
         <v>45488.375</v>
       </c>
-      <c r="D16" s="19"/>
+      <c r="D16" s="18"/>
       <c r="E16" s="10"/>
     </row>
-    <row r="17" ht="15" spans="1:5">
-      <c r="A17" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="B17" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="C17" s="19">
+    <row r="17" spans="1:5">
+      <c r="A17" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" s="18">
         <v>45489.375</v>
       </c>
-      <c r="D17" s="19">
+      <c r="D17" s="18">
         <v>45489.375</v>
       </c>
-      <c r="E17" s="19">
+      <c r="E17" s="18">
         <v>45489.7083333333</v>
       </c>
     </row>
-    <row r="18" ht="15" spans="1:5">
-      <c r="A18" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="B18" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="C18" s="19">
+    <row r="18" spans="1:5">
+      <c r="A18" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" s="18">
         <v>45490.375</v>
       </c>
-      <c r="D18" s="19">
+      <c r="D18" s="18">
         <v>45490.375</v>
       </c>
-      <c r="E18" s="19">
+      <c r="E18" s="18">
         <v>45490.7083333333</v>
       </c>
     </row>
-    <row r="19" ht="15" spans="1:5">
-      <c r="A19" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="B19" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="C19" s="19">
+    <row r="19" spans="1:5">
+      <c r="A19" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" s="18">
         <f>C18+1</f>
         <v>45491.375</v>
       </c>
-      <c r="D19" s="19">
+      <c r="D19" s="18">
         <v>45491.375</v>
       </c>
-      <c r="E19" s="19">
+      <c r="E19" s="18">
         <v>45491.7083333333</v>
       </c>
     </row>
-    <row r="20" ht="15" spans="1:5">
-      <c r="A20" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="B20" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="C20" s="19">
+    <row r="20" spans="1:5">
+      <c r="A20" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" s="18">
         <f t="shared" ref="C20:C32" si="1">C19+1</f>
         <v>45492.375</v>
       </c>
-      <c r="D20" s="19">
+      <c r="D20" s="18">
         <v>45492.375</v>
       </c>
-      <c r="E20" s="19">
+      <c r="E20" s="18">
         <v>45492.7083333333</v>
       </c>
     </row>
-    <row r="21" ht="15" spans="1:5">
-      <c r="A21" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="B21" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="C21" s="19">
+    <row r="21" spans="1:5">
+      <c r="A21" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" s="18">
         <f t="shared" si="1"/>
         <v>45493.375</v>
       </c>
-      <c r="D21" s="19">
+      <c r="D21" s="18">
         <v>45493.375</v>
       </c>
-      <c r="E21" s="19">
+      <c r="E21" s="18">
         <v>45493.7083333333</v>
       </c>
     </row>
-    <row r="22" ht="15" spans="1:5">
-      <c r="A22" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="B22" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="C22" s="19">
+    <row r="22" spans="1:5">
+      <c r="A22" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" s="18">
         <f t="shared" si="1"/>
         <v>45494.375</v>
       </c>
-      <c r="D22" s="19"/>
+      <c r="D22" s="18"/>
       <c r="E22" s="10"/>
     </row>
-    <row r="23" ht="15" spans="1:5">
-      <c r="A23" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="B23" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="C23" s="19">
+    <row r="23" spans="1:5">
+      <c r="A23" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" s="18">
         <f t="shared" si="1"/>
         <v>45495.375</v>
       </c>
-      <c r="D23" s="19">
+      <c r="D23" s="18">
         <v>45495.375</v>
       </c>
-      <c r="E23" s="19">
+      <c r="E23" s="18">
         <v>45495.7083333333</v>
       </c>
     </row>
-    <row r="24" ht="15" spans="1:5">
-      <c r="A24" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="B24" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="C24" s="19">
+    <row r="24" spans="1:5">
+      <c r="A24" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C24" s="18">
         <f t="shared" si="1"/>
         <v>45496.375</v>
       </c>
-      <c r="D24" s="19">
+      <c r="D24" s="18">
         <v>45496.375</v>
       </c>
-      <c r="E24" s="19">
+      <c r="E24" s="18">
         <v>45496.7083333333</v>
       </c>
     </row>
-    <row r="25" ht="15" spans="1:5">
-      <c r="A25" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="B25" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="C25" s="19">
+    <row r="25" spans="1:5">
+      <c r="A25" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B25" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25" s="18">
         <f t="shared" si="1"/>
         <v>45497.375</v>
       </c>
-      <c r="D25" s="19">
+      <c r="D25" s="18">
         <v>45497.375</v>
       </c>
-      <c r="E25" s="19">
+      <c r="E25" s="18">
         <v>45497.7083333333</v>
       </c>
     </row>
-    <row r="26" ht="15" spans="1:5">
-      <c r="A26" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="B26" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="C26" s="19">
+    <row r="26" spans="1:5">
+      <c r="A26" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B26" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C26" s="18">
         <f t="shared" si="1"/>
         <v>45498.375</v>
       </c>
-      <c r="D26" s="19">
+      <c r="D26" s="18">
         <v>45498.375</v>
       </c>
-      <c r="E26" s="19">
+      <c r="E26" s="18">
         <v>45498.7083333333</v>
       </c>
     </row>
-    <row r="27" ht="15" spans="1:5">
-      <c r="A27" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="B27" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="C27" s="19">
+    <row r="27" spans="1:5">
+      <c r="A27" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B27" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C27" s="18">
         <f t="shared" si="1"/>
         <v>45499.375</v>
       </c>
-      <c r="D27" s="19">
+      <c r="D27" s="18">
         <v>45499.375</v>
       </c>
-      <c r="E27" s="19">
+      <c r="E27" s="18">
         <v>45499.7083333333</v>
       </c>
     </row>
-    <row r="28" ht="15" spans="1:5">
-      <c r="A28" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="B28" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="C28" s="19">
+    <row r="28" spans="1:5">
+      <c r="A28" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B28" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C28" s="18">
         <f t="shared" si="1"/>
         <v>45500.375</v>
       </c>
-      <c r="D28" s="19">
+      <c r="D28" s="18">
         <v>45500.375</v>
       </c>
-      <c r="E28" s="19">
+      <c r="E28" s="18">
         <v>45500.7083333333</v>
       </c>
     </row>
-    <row r="29" ht="15" spans="1:5">
-      <c r="A29" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="B29" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="C29" s="19">
+    <row r="29" spans="1:5">
+      <c r="A29" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B29" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C29" s="18">
         <f t="shared" si="1"/>
         <v>45501.375</v>
       </c>
-      <c r="D29" s="19"/>
+      <c r="D29" s="18"/>
       <c r="E29" s="10"/>
     </row>
-    <row r="30" ht="15" spans="1:5">
-      <c r="A30" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="B30" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="C30" s="19">
+    <row r="30" spans="1:5">
+      <c r="A30" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B30" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C30" s="18">
         <f t="shared" si="1"/>
         <v>45502.375</v>
       </c>
-      <c r="D30" s="19">
+      <c r="D30" s="18">
         <v>45502.375</v>
       </c>
-      <c r="E30" s="19">
+      <c r="E30" s="18">
         <v>45502.7083333333</v>
       </c>
     </row>
-    <row r="31" ht="15" spans="1:5">
-      <c r="A31" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="B31" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="C31" s="19">
+    <row r="31" spans="1:5">
+      <c r="A31" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B31" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C31" s="18">
         <f t="shared" si="1"/>
         <v>45503.375</v>
       </c>
-      <c r="D31" s="19">
+      <c r="D31" s="18">
         <v>45503.375</v>
       </c>
-      <c r="E31" s="19">
+      <c r="E31" s="18">
         <v>45503.7083333333</v>
       </c>
     </row>
-    <row r="32" ht="15" spans="1:5">
-      <c r="A32" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="B32" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="C32" s="19">
+    <row r="32" spans="1:5">
+      <c r="A32" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B32" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C32" s="18">
         <f t="shared" si="1"/>
         <v>45504.375</v>
       </c>
-      <c r="D32" s="19">
+      <c r="D32" s="18">
         <v>45504.375</v>
       </c>
-      <c r="E32" s="19">
+      <c r="E32" s="18">
+        <v>45504.7083333333</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C34" s="18">
+        <v>45474.375</v>
+      </c>
+      <c r="D34" s="18"/>
+      <c r="E34" s="10"/>
+      <c r="F34" s="13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C35" s="18">
+        <f t="shared" ref="C35:C47" si="2">C34+1</f>
+        <v>45475.375</v>
+      </c>
+      <c r="D35" s="19"/>
+      <c r="E35" s="19"/>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C36" s="18">
+        <f t="shared" si="2"/>
+        <v>45476.375</v>
+      </c>
+      <c r="D36" s="19"/>
+      <c r="E36" s="19"/>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C37" s="18">
+        <f t="shared" si="2"/>
+        <v>45477.375</v>
+      </c>
+      <c r="D37" s="19"/>
+      <c r="E37" s="19"/>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B38" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C38" s="18">
+        <f t="shared" si="2"/>
+        <v>45478.375</v>
+      </c>
+      <c r="D38" s="19"/>
+      <c r="E38" s="19"/>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B39" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C39" s="18">
+        <f t="shared" si="2"/>
+        <v>45479.375</v>
+      </c>
+      <c r="D39" s="18">
+        <v>45479.5</v>
+      </c>
+      <c r="E39" s="18">
+        <v>45479.7083333333</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B40" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C40" s="18">
+        <f t="shared" si="2"/>
+        <v>45480.375</v>
+      </c>
+      <c r="D40" s="18"/>
+      <c r="E40" s="10"/>
+      <c r="F40" s="13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B41" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C41" s="18">
+        <f t="shared" si="2"/>
+        <v>45481.375</v>
+      </c>
+      <c r="D41" s="18">
+        <v>45481.375</v>
+      </c>
+      <c r="E41" s="18">
+        <v>45481.7083333333</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B42" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C42" s="18">
+        <f t="shared" si="2"/>
+        <v>45482.375</v>
+      </c>
+      <c r="D42" s="18">
+        <v>45482.375</v>
+      </c>
+      <c r="E42" s="18">
+        <v>45482.7083333333</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B43" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C43" s="18">
+        <f t="shared" si="2"/>
+        <v>45483.375</v>
+      </c>
+      <c r="D43" s="18">
+        <v>45483.375</v>
+      </c>
+      <c r="E43" s="18">
+        <v>45483.7083333333</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B44" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C44" s="18">
+        <f t="shared" si="2"/>
+        <v>45484.375</v>
+      </c>
+      <c r="D44" s="18">
+        <v>45484.375</v>
+      </c>
+      <c r="E44" s="18">
+        <v>45484.7083333333</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B45" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C45" s="18">
+        <f t="shared" si="2"/>
+        <v>45485.375</v>
+      </c>
+      <c r="D45" s="18">
+        <v>45485.375</v>
+      </c>
+      <c r="E45" s="18">
+        <v>45485.7083333333</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B46" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C46" s="18">
+        <f t="shared" si="2"/>
+        <v>45486.375</v>
+      </c>
+      <c r="D46" s="18">
+        <v>45486.375</v>
+      </c>
+      <c r="E46" s="18">
+        <v>45486.7083333333</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B47" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C47" s="18">
+        <f t="shared" si="2"/>
+        <v>45487.375</v>
+      </c>
+      <c r="D47" s="18">
+        <v>45487.375</v>
+      </c>
+      <c r="E47" s="18">
+        <v>45487.7083333333</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
+      <c r="A48" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B48" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C48" s="18">
+        <v>45488.375</v>
+      </c>
+      <c r="D48" s="18"/>
+      <c r="E48" s="10"/>
+      <c r="F48" s="13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B49" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C49" s="18">
+        <v>45489.375</v>
+      </c>
+      <c r="D49" s="18">
+        <v>45489.375</v>
+      </c>
+      <c r="E49" s="18">
+        <v>45489.7083333333</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B50" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C50" s="18">
+        <v>45490.375</v>
+      </c>
+      <c r="D50" s="18">
+        <v>45490.375</v>
+      </c>
+      <c r="E50" s="18">
+        <v>45490.7083333333</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B51" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C51" s="18">
+        <f t="shared" ref="C51:C64" si="3">C50+1</f>
+        <v>45491.375</v>
+      </c>
+      <c r="D51" s="18">
+        <v>45491.375</v>
+      </c>
+      <c r="E51" s="18">
+        <v>45491.7083333333</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B52" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C52" s="18">
+        <f t="shared" si="3"/>
+        <v>45492.375</v>
+      </c>
+      <c r="D52" s="18">
+        <v>45492.375</v>
+      </c>
+      <c r="E52" s="18">
+        <v>45492.7083333333</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B53" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C53" s="18">
+        <f t="shared" si="3"/>
+        <v>45493.375</v>
+      </c>
+      <c r="D53" s="18">
+        <v>45493.375</v>
+      </c>
+      <c r="E53" s="18">
+        <v>45493.7083333333</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6">
+      <c r="A54" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B54" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C54" s="18">
+        <f t="shared" si="3"/>
+        <v>45494.375</v>
+      </c>
+      <c r="D54" s="18"/>
+      <c r="E54" s="10"/>
+      <c r="F54" s="13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B55" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C55" s="18">
+        <f t="shared" si="3"/>
+        <v>45495.375</v>
+      </c>
+      <c r="D55" s="18">
+        <v>45495.375</v>
+      </c>
+      <c r="E55" s="18">
+        <v>45495.7083333333</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="A56" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B56" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C56" s="18">
+        <f t="shared" si="3"/>
+        <v>45496.375</v>
+      </c>
+      <c r="D56" s="18">
+        <v>45496.375</v>
+      </c>
+      <c r="E56" s="18">
+        <v>45496.7083333333</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="A57" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B57" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C57" s="18">
+        <f t="shared" si="3"/>
+        <v>45497.375</v>
+      </c>
+      <c r="D57" s="18">
+        <v>45497.375</v>
+      </c>
+      <c r="E57" s="18">
+        <v>45497.7083333333</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
+      <c r="A58" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B58" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C58" s="18">
+        <f t="shared" si="3"/>
+        <v>45498.375</v>
+      </c>
+      <c r="D58" s="18">
+        <v>45498.375</v>
+      </c>
+      <c r="E58" s="18">
+        <v>45498.7083333333</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
+      <c r="A59" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B59" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C59" s="18">
+        <f t="shared" si="3"/>
+        <v>45499.375</v>
+      </c>
+      <c r="D59" s="18">
+        <v>45499.375</v>
+      </c>
+      <c r="E59" s="18">
+        <v>45499.7083333333</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
+      <c r="A60" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B60" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C60" s="18">
+        <f t="shared" si="3"/>
+        <v>45500.375</v>
+      </c>
+      <c r="D60" s="18">
+        <v>45500.375</v>
+      </c>
+      <c r="E60" s="18">
+        <v>45500.7083333333</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6">
+      <c r="A61" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B61" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C61" s="18">
+        <f t="shared" si="3"/>
+        <v>45501.375</v>
+      </c>
+      <c r="D61" s="18"/>
+      <c r="E61" s="10"/>
+      <c r="F61" s="13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="A62" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B62" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C62" s="18">
+        <f t="shared" si="3"/>
+        <v>45502.375</v>
+      </c>
+      <c r="D62" s="18">
+        <v>45502.375</v>
+      </c>
+      <c r="E62" s="18">
+        <v>45502.7083333333</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="A63" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B63" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C63" s="18">
+        <f t="shared" si="3"/>
+        <v>45503.375</v>
+      </c>
+      <c r="D63" s="18">
+        <v>45503.375</v>
+      </c>
+      <c r="E63" s="18">
+        <v>45503.7083333333</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
+      <c r="A64" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B64" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C64" s="18">
+        <f t="shared" si="3"/>
+        <v>45504.375</v>
+      </c>
+      <c r="D64" s="18">
+        <v>45504.375</v>
+      </c>
+      <c r="E64" s="18">
         <v>45504.7083333333</v>
       </c>
     </row>
@@ -1655,16 +2219,16 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A7" sqref="A7:B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="6"/>
   <cols>
-    <col min="1" max="1" width="12.4333333333333" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.7166666666667" style="2" customWidth="1"/>
-    <col min="3" max="3" width="12.4333333333333" style="3" customWidth="1"/>
-    <col min="4" max="6" width="16.8583333333333" style="2" customWidth="1"/>
-    <col min="7" max="7" width="12.4333333333333" style="2" customWidth="1"/>
+    <col min="1" max="1" width="12.4296875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.71875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="12.4296875" style="3" customWidth="1"/>
+    <col min="4" max="6" width="16.859375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="12.4296875" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="17.25" customHeight="1" spans="1:4">
@@ -1675,10 +2239,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:5">
@@ -1692,7 +2256,7 @@
         <v>45494</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E2" s="10"/>
     </row>
@@ -1707,7 +2271,7 @@
         <v>45501</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" ht="17.25" customHeight="1" spans="1:4">
@@ -1721,7 +2285,7 @@
         <v>45480</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" ht="17.25" customHeight="1" spans="1:4">
@@ -1735,17 +2299,66 @@
         <v>45488</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" ht="17.25" customHeight="1"/>
-    <row r="7" ht="17.25" customHeight="1" spans="7:7">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" ht="17.25" customHeight="1" spans="1:4">
+      <c r="A6" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="9">
+        <v>45475</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" ht="17.25" customHeight="1" spans="1:7">
+      <c r="A7" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="9">
+        <v>45476</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="G7" s="9"/>
     </row>
-    <row r="8" ht="17.25" customHeight="1" spans="7:7">
+    <row r="8" ht="17.25" customHeight="1" spans="1:7">
+      <c r="A8" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="9">
+        <v>45477</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="G8" s="9"/>
     </row>
-    <row r="9" ht="17.25" customHeight="1" spans="7:7">
+    <row r="9" ht="17.25" customHeight="1" spans="1:7">
+      <c r="A9" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="9">
+        <v>45478</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="G9" s="9"/>
     </row>
   </sheetData>

</xml_diff>